<commit_message>
Oppdatering, jobber videre med statistikk funksjon
</commit_message>
<xml_diff>
--- a/EasyTimeWebApp/public/files/marinaden.xlsx
+++ b/EasyTimeWebApp/public/files/marinaden.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Tid</t>
   </si>
@@ -25,73 +25,40 @@
     <t>Dato</t>
   </si>
   <si>
-    <t>10.30</t>
+    <t>10-17.00</t>
   </si>
   <si>
     <t>Marius Sørenes</t>
   </si>
   <si>
-    <t>27.07.2016</t>
-  </si>
-  <si>
-    <t>16.00</t>
+    <t>02.08.2016</t>
+  </si>
+  <si>
+    <t>18.00</t>
   </si>
   <si>
     <t>Johannes Steinsbø</t>
   </si>
   <si>
-    <t>18.00</t>
-  </si>
-  <si>
-    <t>18.02</t>
-  </si>
-  <si>
-    <t>08.00</t>
-  </si>
-  <si>
-    <t>28.07.2016</t>
-  </si>
-  <si>
-    <t>09.00</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>Bergliot Olavsen</t>
-  </si>
-  <si>
-    <t>11.00</t>
-  </si>
-  <si>
-    <t>29.07.2016</t>
-  </si>
-  <si>
-    <t>12.00</t>
-  </si>
-  <si>
-    <t>Jon Olav</t>
-  </si>
-  <si>
-    <t>13.00</t>
-  </si>
-  <si>
-    <t>Nessen</t>
-  </si>
-  <si>
-    <t>14.00</t>
-  </si>
-  <si>
-    <t>Sigmund Steinsbø</t>
+    <t>01.08.2016</t>
+  </si>
+  <si>
+    <t>John Stone</t>
+  </si>
+  <si>
+    <t>Mafr Brt</t>
+  </si>
+  <si>
+    <t>31.07.2016</t>
+  </si>
+  <si>
+    <t>06-17.00</t>
+  </si>
+  <si>
+    <t>Kristian Sortland</t>
   </si>
   <si>
     <t>30.07.2016</t>
-  </si>
-  <si>
-    <t>15.00</t>
-  </si>
-  <si>
-    <t>Ola Nordmann</t>
   </si>
 </sst>
 </file>
@@ -468,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -509,37 +476,37 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -547,90 +514,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdatering, lagd til demo av Tidsberekning til plot.py
</commit_message>
<xml_diff>
--- a/EasyTimeWebApp/public/files/marinaden.xlsx
+++ b/EasyTimeWebApp/public/files/marinaden.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Tid</t>
   </si>
@@ -25,40 +25,64 @@
     <t>Dato</t>
   </si>
   <si>
-    <t>10-17.00</t>
+    <t>10.30</t>
   </si>
   <si>
     <t>Marius Sørenes</t>
   </si>
   <si>
-    <t>02.08.2016</t>
+    <t>27.07.2016</t>
+  </si>
+  <si>
+    <t>16.00</t>
+  </si>
+  <si>
+    <t>Johannes  Steinsbø</t>
   </si>
   <si>
     <t>18.00</t>
   </si>
   <si>
-    <t>Johannes Steinsbø</t>
-  </si>
-  <si>
-    <t>01.08.2016</t>
-  </si>
-  <si>
-    <t>John Stone</t>
-  </si>
-  <si>
-    <t>Mafr Brt</t>
-  </si>
-  <si>
-    <t>31.07.2016</t>
-  </si>
-  <si>
-    <t>06-17.00</t>
-  </si>
-  <si>
-    <t>Kristian Sortland</t>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>Bergliot  Olavsen</t>
+  </si>
+  <si>
+    <t>28.07.2016</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>29.07.2016</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>Jon  Olav</t>
+  </si>
+  <si>
+    <t>13.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessen </t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>Sigmund  Steinsbø</t>
   </si>
   <si>
     <t>30.07.2016</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>Ola  Nordmann</t>
   </si>
 </sst>
 </file>
@@ -435,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -476,23 +500,23 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -506,32 +530,54 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>